<commit_message>
Changes to final ms, adding figure describing analysis path
</commit_message>
<xml_diff>
--- a/Manuscript/Table1.xlsx
+++ b/Manuscript/Table1.xlsx
@@ -365,17 +365,17 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Symbol</t>
+          <t>Remained Occupied</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>First Visit</t>
+          <t>Extirpated</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Second Visit</t>
+          <t>Colonized</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -395,16 +395,14 @@
           <t>*Abies amabilis*</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>ABAM</t>
-        </is>
+      <c r="B2">
+        <v>1130</v>
       </c>
       <c r="C2">
-        <v>1163</v>
+        <v>33</v>
       </c>
       <c r="D2">
-        <v>1171</v>
+        <v>41</v>
       </c>
       <c r="E2">
         <v>365</v>
@@ -419,16 +417,14 @@
           <t>*Abies concolor*</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ABCO</t>
-        </is>
+      <c r="B3">
+        <v>1874</v>
       </c>
       <c r="C3">
-        <v>2016</v>
+        <v>142</v>
       </c>
       <c r="D3">
-        <v>1954</v>
+        <v>80</v>
       </c>
       <c r="E3">
         <v>752</v>
@@ -443,16 +439,14 @@
           <t>*Abies grandis*</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>ABGR</t>
-        </is>
+      <c r="B4">
+        <v>1642</v>
       </c>
       <c r="C4">
-        <v>1768</v>
+        <v>126</v>
       </c>
       <c r="D4">
-        <v>1754</v>
+        <v>112</v>
       </c>
       <c r="E4">
         <v>544</v>
@@ -467,16 +461,14 @@
           <t>*Abies lasiocarpa*</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>ABLA</t>
-        </is>
+      <c r="B5">
+        <v>684</v>
       </c>
       <c r="C5">
-        <v>774</v>
+        <v>90</v>
       </c>
       <c r="D5">
-        <v>723</v>
+        <v>39</v>
       </c>
       <c r="E5">
         <v>320</v>
@@ -491,16 +483,14 @@
           <t>*Abies magnifica*</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>ABMA</t>
-        </is>
+      <c r="B6">
+        <v>561</v>
       </c>
       <c r="C6">
-        <v>579</v>
+        <v>18</v>
       </c>
       <c r="D6">
-        <v>582</v>
+        <v>21</v>
       </c>
       <c r="E6">
         <v>200</v>
@@ -515,16 +505,14 @@
           <t>*Abies procera*</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>ABPR</t>
-        </is>
+      <c r="B7">
+        <v>383</v>
       </c>
       <c r="C7">
-        <v>401</v>
+        <v>18</v>
       </c>
       <c r="D7">
-        <v>423</v>
+        <v>40</v>
       </c>
       <c r="E7">
         <v>83</v>
@@ -539,16 +527,14 @@
           <t>*Chamaecyparis lawsoniana*</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>CHLA</t>
-        </is>
+      <c r="B8">
+        <v>77</v>
       </c>
       <c r="C8">
-        <v>85</v>
+        <v>8</v>
       </c>
       <c r="D8">
-        <v>81</v>
+        <v>4</v>
       </c>
       <c r="E8">
         <v>17</v>
@@ -563,16 +549,14 @@
           <t>*Chamaecyparis nootkatensis*</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>CHNO</t>
-        </is>
+      <c r="B9">
+        <v>110</v>
       </c>
       <c r="C9">
-        <v>112</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>116</v>
+        <v>6</v>
       </c>
       <c r="E9">
         <v>24</v>
@@ -587,16 +571,14 @@
           <t>*Juniperus californica*</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>JUCA7</t>
-        </is>
+      <c r="B10">
+        <v>62</v>
       </c>
       <c r="C10">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <v>5</v>
@@ -611,16 +593,14 @@
           <t>*Juniperus occidentalis*</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>JUOC</t>
-        </is>
+      <c r="B11">
+        <v>965</v>
       </c>
       <c r="C11">
-        <v>1020</v>
+        <v>55</v>
       </c>
       <c r="D11">
-        <v>1013</v>
+        <v>48</v>
       </c>
       <c r="E11">
         <v>130</v>
@@ -635,16 +615,14 @@
           <t>*Larix occidentalis*</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>LAOC</t>
-        </is>
+      <c r="B12">
+        <v>985</v>
       </c>
       <c r="C12">
-        <v>1059</v>
+        <v>74</v>
       </c>
       <c r="D12">
-        <v>1056</v>
+        <v>71</v>
       </c>
       <c r="E12">
         <v>278</v>
@@ -659,16 +637,14 @@
           <t>*Calocedrus decurrens*</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>CADE27</t>
-        </is>
+      <c r="B13">
+        <v>1240</v>
       </c>
       <c r="C13">
-        <v>1329</v>
+        <v>89</v>
       </c>
       <c r="D13">
-        <v>1302</v>
+        <v>62</v>
       </c>
       <c r="E13">
         <v>309</v>
@@ -683,16 +659,14 @@
           <t>*Picea engelmannii*</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>PIEN</t>
-        </is>
+      <c r="B14">
+        <v>658</v>
       </c>
       <c r="C14">
-        <v>749</v>
+        <v>91</v>
       </c>
       <c r="D14">
-        <v>704</v>
+        <v>46</v>
       </c>
       <c r="E14">
         <v>221</v>
@@ -707,16 +681,14 @@
           <t>*Picea sitchensis*</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>PISI</t>
-        </is>
+      <c r="B15">
+        <v>233</v>
       </c>
       <c r="C15">
-        <v>269</v>
+        <v>36</v>
       </c>
       <c r="D15">
-        <v>261</v>
+        <v>28</v>
       </c>
       <c r="E15">
         <v>92</v>
@@ -731,16 +703,14 @@
           <t>*Pinus albicaulis*</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>PIAL</t>
-        </is>
+      <c r="B16">
+        <v>173</v>
       </c>
       <c r="C16">
-        <v>203</v>
+        <v>30</v>
       </c>
       <c r="D16">
-        <v>181</v>
+        <v>8</v>
       </c>
       <c r="E16">
         <v>77</v>
@@ -755,16 +725,14 @@
           <t>*Pinus attenuata*</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>PIAT</t>
-        </is>
+      <c r="B17">
+        <v>61</v>
       </c>
       <c r="C17">
-        <v>83</v>
+        <v>22</v>
       </c>
       <c r="D17">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="E17">
         <v>43</v>
@@ -779,16 +747,14 @@
           <t>*Pinus contorta*</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>PICO</t>
-        </is>
+      <c r="B18">
+        <v>2058</v>
       </c>
       <c r="C18">
-        <v>2255</v>
+        <v>198</v>
       </c>
       <c r="D18">
-        <v>2193</v>
+        <v>135</v>
       </c>
       <c r="E18">
         <v>885</v>
@@ -803,16 +769,14 @@
           <t>*Pinus jeffreyi*</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>PIJE</t>
-        </is>
+      <c r="B19">
+        <v>608</v>
       </c>
       <c r="C19">
-        <v>637</v>
+        <v>29</v>
       </c>
       <c r="D19">
-        <v>622</v>
+        <v>14</v>
       </c>
       <c r="E19">
         <v>144</v>
@@ -827,16 +791,14 @@
           <t>*Pinus lambertiana*</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>PILA</t>
-        </is>
+      <c r="B20">
+        <v>876</v>
       </c>
       <c r="C20">
-        <v>991</v>
+        <v>115</v>
       </c>
       <c r="D20">
-        <v>914</v>
+        <v>38</v>
       </c>
       <c r="E20">
         <v>227</v>
@@ -851,16 +813,14 @@
           <t>*Pinus monticola*</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>PIMO3</t>
-        </is>
+      <c r="B21">
+        <v>538</v>
       </c>
       <c r="C21">
-        <v>604</v>
+        <v>66</v>
       </c>
       <c r="D21">
-        <v>605</v>
+        <v>67</v>
       </c>
       <c r="E21">
         <v>159</v>
@@ -875,16 +835,14 @@
           <t>*Pinus ponderosa*</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>PIPO</t>
-        </is>
+      <c r="B22">
+        <v>4374</v>
       </c>
       <c r="C22">
-        <v>4581</v>
+        <v>207</v>
       </c>
       <c r="D22">
-        <v>4606</v>
+        <v>232</v>
       </c>
       <c r="E22">
         <v>1238</v>
@@ -899,16 +857,14 @@
           <t>*Pinus sabiniana*</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>PISA2</t>
-        </is>
+      <c r="B23">
+        <v>171</v>
       </c>
       <c r="C23">
-        <v>195</v>
+        <v>24</v>
       </c>
       <c r="D23">
-        <v>185</v>
+        <v>14</v>
       </c>
       <c r="E23">
         <v>41</v>
@@ -923,16 +879,14 @@
           <t>*Pinus monophylla*</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>PIMO</t>
-        </is>
+      <c r="B24">
+        <v>190</v>
       </c>
       <c r="C24">
-        <v>203</v>
+        <v>13</v>
       </c>
       <c r="D24">
-        <v>193</v>
+        <v>3</v>
       </c>
       <c r="E24">
         <v>56</v>
@@ -947,16 +901,14 @@
           <t>*Pseudotsuga menziesii*</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>PSME</t>
-        </is>
+      <c r="B25">
+        <v>7898</v>
       </c>
       <c r="C25">
-        <v>8269</v>
+        <v>371</v>
       </c>
       <c r="D25">
-        <v>8258</v>
+        <v>360</v>
       </c>
       <c r="E25">
         <v>2673</v>
@@ -971,16 +923,14 @@
           <t>*Sequoia sempervirens*</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>SESE3</t>
-        </is>
+      <c r="B26">
+        <v>238</v>
       </c>
       <c r="C26">
-        <v>240</v>
+        <v>2</v>
       </c>
       <c r="D26">
-        <v>242</v>
+        <v>4</v>
       </c>
       <c r="E26">
         <v>48</v>
@@ -995,16 +945,14 @@
           <t>*Taxus brevifolia*</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>TABR2</t>
-        </is>
+      <c r="B27">
+        <v>195</v>
       </c>
       <c r="C27">
-        <v>220</v>
+        <v>25</v>
       </c>
       <c r="D27">
-        <v>206</v>
+        <v>11</v>
       </c>
       <c r="E27">
         <v>44</v>
@@ -1019,16 +967,14 @@
           <t>*Thuja plicata*</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>THPL</t>
-        </is>
+      <c r="B28">
+        <v>1388</v>
       </c>
       <c r="C28">
-        <v>1461</v>
+        <v>73</v>
       </c>
       <c r="D28">
-        <v>1487</v>
+        <v>99</v>
       </c>
       <c r="E28">
         <v>220</v>
@@ -1043,16 +989,14 @@
           <t>*Tsuga heterophylla*</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>TSHE</t>
-        </is>
+      <c r="B29">
+        <v>2585</v>
       </c>
       <c r="C29">
-        <v>2745</v>
+        <v>160</v>
       </c>
       <c r="D29">
-        <v>2788</v>
+        <v>203</v>
       </c>
       <c r="E29">
         <v>823</v>
@@ -1067,16 +1011,14 @@
           <t>*Tsuga mertensiana*</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>TSME</t>
-        </is>
+      <c r="B30">
+        <v>724</v>
       </c>
       <c r="C30">
-        <v>743</v>
+        <v>19</v>
       </c>
       <c r="D30">
-        <v>754</v>
+        <v>30</v>
       </c>
       <c r="E30">
         <v>184</v>
@@ -1091,16 +1033,14 @@
           <t>*Acer macrophyllum*</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>ACMA3</t>
-        </is>
+      <c r="B31">
+        <v>853</v>
       </c>
       <c r="C31">
-        <v>941</v>
+        <v>88</v>
       </c>
       <c r="D31">
-        <v>941</v>
+        <v>88</v>
       </c>
       <c r="E31">
         <v>237</v>
@@ -1115,16 +1055,14 @@
           <t>*Aesculus californica*</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>AECA</t>
-        </is>
+      <c r="B32">
+        <v>69</v>
       </c>
       <c r="C32">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="D32">
-        <v>74</v>
+        <v>5</v>
       </c>
       <c r="E32">
         <v>25</v>
@@ -1139,16 +1077,14 @@
           <t>*Alnus rubra*</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>ALRU2</t>
-        </is>
+      <c r="B33">
+        <v>1128</v>
       </c>
       <c r="C33">
-        <v>1318</v>
+        <v>190</v>
       </c>
       <c r="D33">
-        <v>1286</v>
+        <v>158</v>
       </c>
       <c r="E33">
         <v>663</v>
@@ -1163,16 +1099,14 @@
           <t>*Alnus rhombifolia*</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>ALRH2</t>
-        </is>
+      <c r="B34">
+        <v>63</v>
       </c>
       <c r="C34">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="D34">
-        <v>66</v>
+        <v>3</v>
       </c>
       <c r="E34">
         <v>28</v>
@@ -1187,16 +1121,14 @@
           <t>*Arbutus menziesii*</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>ARME</t>
-        </is>
+      <c r="B35">
+        <v>754</v>
       </c>
       <c r="C35">
-        <v>839</v>
+        <v>85</v>
       </c>
       <c r="D35">
-        <v>803</v>
+        <v>49</v>
       </c>
       <c r="E35">
         <v>314</v>
@@ -1211,16 +1143,14 @@
           <t>*Betula papyrifera*</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>BEPA</t>
-        </is>
+      <c r="B36">
+        <v>66</v>
       </c>
       <c r="C36">
-        <v>80</v>
+        <v>14</v>
       </c>
       <c r="D36">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="E36">
         <v>45</v>
@@ -1235,16 +1165,14 @@
           <t>*Chrysolepis chrysophylla*</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>CHCHC4</t>
-        </is>
+      <c r="B37">
+        <v>289</v>
       </c>
       <c r="C37">
-        <v>345</v>
+        <v>56</v>
       </c>
       <c r="D37">
-        <v>328</v>
+        <v>39</v>
       </c>
       <c r="E37">
         <v>120</v>
@@ -1259,16 +1187,14 @@
           <t>*Cornus nuttallii*</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>CONU4</t>
-        </is>
+      <c r="B38">
+        <v>66</v>
       </c>
       <c r="C38">
-        <v>95</v>
+        <v>29</v>
       </c>
       <c r="D38">
-        <v>84</v>
+        <v>18</v>
       </c>
       <c r="E38">
         <v>30</v>
@@ -1283,16 +1209,14 @@
           <t>*Fraxinus latifolia*</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>FRLA</t>
-        </is>
+      <c r="B39">
+        <v>54</v>
       </c>
       <c r="C39">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="D39">
-        <v>65</v>
+        <v>11</v>
       </c>
       <c r="E39">
         <v>13</v>
@@ -1307,16 +1231,14 @@
           <t>*Notholithocarpus densiflorus*</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>NODE3</t>
-        </is>
+      <c r="B40">
+        <v>611</v>
       </c>
       <c r="C40">
-        <v>650</v>
+        <v>39</v>
       </c>
       <c r="D40">
-        <v>643</v>
+        <v>32</v>
       </c>
       <c r="E40">
         <v>279</v>
@@ -1331,16 +1253,14 @@
           <t>*Populus tremuloides*</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>POTR5</t>
-        </is>
+      <c r="B41">
+        <v>98</v>
       </c>
       <c r="C41">
-        <v>119</v>
+        <v>21</v>
       </c>
       <c r="D41">
-        <v>106</v>
+        <v>8</v>
       </c>
       <c r="E41">
         <v>60</v>
@@ -1355,16 +1275,14 @@
           <t>*Populus balsamifera*</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>POBAT</t>
-        </is>
+      <c r="B42">
+        <v>149</v>
       </c>
       <c r="C42">
-        <v>168</v>
+        <v>19</v>
       </c>
       <c r="D42">
-        <v>167</v>
+        <v>18</v>
       </c>
       <c r="E42">
         <v>30</v>
@@ -1379,16 +1297,14 @@
           <t>*Quercus agrifolia*</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>QUAG</t>
-        </is>
+      <c r="B43">
+        <v>188</v>
       </c>
       <c r="C43">
-        <v>199</v>
+        <v>11</v>
       </c>
       <c r="D43">
-        <v>194</v>
+        <v>6</v>
       </c>
       <c r="E43">
         <v>65</v>
@@ -1403,16 +1319,14 @@
           <t>*Quercus chrysolepis*</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>QUCH2</t>
-        </is>
+      <c r="B44">
+        <v>791</v>
       </c>
       <c r="C44">
-        <v>851</v>
+        <v>60</v>
       </c>
       <c r="D44">
-        <v>821</v>
+        <v>30</v>
       </c>
       <c r="E44">
         <v>228</v>
@@ -1427,16 +1341,14 @@
           <t>*Quercus douglasii*</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>QUDO</t>
-        </is>
+      <c r="B45">
+        <v>335</v>
       </c>
       <c r="C45">
-        <v>340</v>
+        <v>5</v>
       </c>
       <c r="D45">
-        <v>335</v>
+        <v>0</v>
       </c>
       <c r="E45">
         <v>68</v>
@@ -1451,16 +1363,14 @@
           <t>*Quercus garryana*</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>QUGA4</t>
-        </is>
+      <c r="B46">
+        <v>321</v>
       </c>
       <c r="C46">
-        <v>334</v>
+        <v>13</v>
       </c>
       <c r="D46">
-        <v>332</v>
+        <v>11</v>
       </c>
       <c r="E46">
         <v>89</v>
@@ -1475,16 +1385,14 @@
           <t>*Quercus kelloggii*</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>QUKE</t>
-        </is>
+      <c r="B47">
+        <v>805</v>
       </c>
       <c r="C47">
-        <v>896</v>
+        <v>91</v>
       </c>
       <c r="D47">
-        <v>847</v>
+        <v>42</v>
       </c>
       <c r="E47">
         <v>327</v>
@@ -1499,16 +1407,14 @@
           <t>*Quercus lobata*</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>QULO</t>
-        </is>
+      <c r="B48">
+        <v>60</v>
       </c>
       <c r="C48">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="D48">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="E48">
         <v>9</v>
@@ -1523,16 +1429,14 @@
           <t>*Quercus wislizeni*</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>QUWI2</t>
-        </is>
+      <c r="B49">
+        <v>184</v>
       </c>
       <c r="C49">
-        <v>207</v>
+        <v>23</v>
       </c>
       <c r="D49">
-        <v>197</v>
+        <v>13</v>
       </c>
       <c r="E49">
         <v>86</v>
@@ -1547,16 +1451,14 @@
           <t>*Umbellularia californica*</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>UMCA</t>
-        </is>
+      <c r="B50">
+        <v>256</v>
       </c>
       <c r="C50">
-        <v>264</v>
+        <v>8</v>
       </c>
       <c r="D50">
-        <v>277</v>
+        <v>21</v>
       </c>
       <c r="E50">
         <v>39</v>

</xml_diff>